<commit_message>
change the order of experience
</commit_message>
<xml_diff>
--- a/data/cv.xlsx
+++ b/data/cv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/259d7e333b35feb4/Frank/CV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="8_{5A14CAED-B1A4-469F-8095-BE08698611DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5E449F6-213B-4FC6-A80B-4FF9D7EE2FCE}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{5A14CAED-B1A4-469F-8095-BE08698611DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AD03CFF-5C42-448B-81D5-96000C6851EA}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contact" sheetId="1" r:id="rId1"/>
@@ -914,7 +914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
@@ -1425,8 +1425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1459,44 +1459,44 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>140</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>133</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>138</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
         <v>139</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>162</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>165</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C3" t="s">
-        <v>167</v>
-      </c>
-      <c r="D3" t="s">
-        <v>168</v>
-      </c>
-      <c r="E3" t="s">
-        <v>138</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -1556,6 +1556,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>